<commit_message>
Update Read Excel Code
</commit_message>
<xml_diff>
--- a/test-output/ExcelReports/GenericTestOutput.xlsx
+++ b/test-output/ExcelReports/GenericTestOutput.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="25">
   <si>
     <t>URL</t>
   </si>
@@ -108,13 +108,63 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -167,11 +217,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,108 +592,108 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="17" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>